<commit_message>
* Started yet another renderer * Consolidated some of the similarities between the pixel and z buffer classes into a base abstract class
</commit_message>
<xml_diff>
--- a/jdem846/resources/Pixel Buffer Memory Calculations.xlsx
+++ b/jdem846/resources/Pixel Buffer Memory Calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19020" windowHeight="11070"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19020" windowHeight="11070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Width:</t>
   </si>
@@ -58,6 +58,51 @@
   </si>
   <si>
     <t>int:</t>
+  </si>
+  <si>
+    <t>Total Points:</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>double[3]</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Size:</t>
+  </si>
+  <si>
+    <t>Elevation:</t>
+  </si>
+  <si>
+    <t>Normal:</t>
+  </si>
+  <si>
+    <t>Dot Product:</t>
+  </si>
+  <si>
+    <t>RGBA:</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>Subpixel Grid:</t>
+  </si>
+  <si>
+    <t>Total Model Size:</t>
+  </si>
+  <si>
+    <t>Total Image Size:</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Total Memory Size:</t>
   </si>
 </sst>
 </file>
@@ -69,7 +114,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +162,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -139,7 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -159,6 +212,22 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -579,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,16 +1020,277 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3">
+        <f>B1*B2</f>
+        <v>2250000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="A6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="17">
+        <f>B3*B5</f>
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="13">
+        <f>SUM(C9:C12)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4">
+        <f>B6*C13</f>
+        <v>396000000</v>
+      </c>
+      <c r="C16" s="5">
+        <f>B16/POWER(2, 20)</f>
+        <v>377.655029296875</v>
+      </c>
+      <c r="D16" s="5">
+        <f>B16/POWER(2, 30)</f>
+        <v>0.36880373954772949</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="3">
+        <f>B6 * B19</f>
+        <v>36000000</v>
+      </c>
+      <c r="C23" s="11">
+        <f>B23/POWER(2, 20)</f>
+        <v>34.332275390625</v>
+      </c>
+      <c r="D23" s="11">
+        <f>B23/POWER(2, 30)</f>
+        <v>3.3527612686157227E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3">
+        <f>B6*B20</f>
+        <v>72000000</v>
+      </c>
+      <c r="C24" s="11">
+        <f>B24/POWER(2, 20)</f>
+        <v>68.66455078125</v>
+      </c>
+      <c r="D24" s="11">
+        <f>B24/POWER(2, 30)</f>
+        <v>6.7055225372314453E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="4">
+        <f>B23+B24</f>
+        <v>108000000</v>
+      </c>
+      <c r="C26" s="5">
+        <f>B26/POWER(2, 20)</f>
+        <v>102.996826171875</v>
+      </c>
+      <c r="D26" s="5">
+        <f>B26/POWER(2, 30)</f>
+        <v>0.10058283805847168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="21">
+        <f>B16+B26</f>
+        <v>504000000</v>
+      </c>
+      <c r="C30" s="22">
+        <f>B30/POWER(2, 20)</f>
+        <v>480.65185546875</v>
+      </c>
+      <c r="D30" s="22">
+        <f>B30/POWER(2, 30)</f>
+        <v>0.46938657760620117</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>